<commit_message>
Add notebook for the model and training
</commit_message>
<xml_diff>
--- a/real_life_playing/human_results/game1.xlsx
+++ b/real_life_playing/human_results/game1.xlsx
@@ -5137,27 +5137,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Artificial Player</t>
+          <t>Francesco</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Francesco</t>
+          <t>Camilla</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Camilla</t>
+          <t>Artificial Player</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>